<commit_message>
With this commit, I made some edits to the 2019/20 file
</commit_message>
<xml_diff>
--- a/2019_20_sample.xlsx
+++ b/2019_20_sample.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/2e6d500d54c3f689/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ganiy\OneDrive\Documents\DSI-SRP1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1CEB8661-4981-4CDE-A0C6-FCB1DC720B4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="8_{1CEB8661-4981-4CDE-A0C6-FCB1DC720B4E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{4F8EE93F-A19A-4584-B04C-CF3E659EE593}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{3D70B543-D19F-4DC0-8523-1DD73DC427EB}"/>
   </bookViews>
@@ -57,9 +57,6 @@
     <t>fpl_to_game</t>
   </si>
   <si>
-    <t>Keita</t>
-  </si>
-  <si>
     <t>Alisson</t>
   </si>
   <si>
@@ -121,6 +118,9 @@
   </si>
   <si>
     <t>Vardy</t>
+  </si>
+  <si>
+    <t>Fabinho</t>
   </si>
 </sst>
 </file>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2289137D-01D2-468F-8ECB-96BBA888633F}">
   <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -517,7 +517,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -544,7 +544,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -598,7 +598,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -625,7 +625,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -679,7 +679,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>4</v>
@@ -706,7 +706,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -733,7 +733,7 @@
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -760,7 +760,7 @@
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11">
         <v>0</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B12">
         <v>1</v>
@@ -814,34 +814,34 @@
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="B13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13">
         <v>3</v>
       </c>
       <c r="D13">
-        <v>666</v>
+        <v>1989</v>
       </c>
       <c r="E13">
         <v>3</v>
       </c>
       <c r="F13">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G13">
-        <v>43</v>
+        <v>75</v>
       </c>
       <c r="H13">
         <f t="shared" si="0"/>
-        <v>5.8108108108108114</v>
+        <v>3.3936651583710407</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B14">
         <v>4</v>
@@ -868,7 +868,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -895,7 +895,7 @@
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B16">
         <v>7</v>
@@ -922,7 +922,7 @@
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B17">
         <v>17</v>
@@ -949,7 +949,7 @@
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18">
         <v>5</v>
@@ -976,7 +976,7 @@
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19">
         <v>19</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>12</v>
@@ -1030,7 +1030,7 @@
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B21">
         <v>8</v>
@@ -1057,7 +1057,7 @@
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B22">
         <v>2</v>
@@ -1084,7 +1084,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B23">
         <v>23</v>

</xml_diff>